<commit_message>
updated regn and login test
updated regn and login test
</commit_message>
<xml_diff>
--- a/DSAlgoProject/src/test/resources/InputData.xlsx
+++ b/DSAlgoProject/src/test/resources/InputData.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="signIn" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="registerPg" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="31">
   <si>
     <t xml:space="preserve">userId</t>
   </si>
@@ -32,30 +32,97 @@
     <t xml:space="preserve">expectedResult</t>
   </si>
   <si>
+    <t xml:space="preserve">Cases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pwd@1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid</t>
+  </si>
+  <si>
     <t xml:space="preserve">Priya.Acharya</t>
   </si>
   <si>
-    <t xml:space="preserve">Pwd@1234</t>
+    <t xml:space="preserve">Priya_Acharya3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pwd@12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid Username and Password</t>
   </si>
   <si>
     <t xml:space="preserve">You are logged in</t>
   </si>
   <si>
-    <t xml:space="preserve">Pwd@12345</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Invalid Username and Password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Priya_Acharya3</t>
+    <t xml:space="preserve">Valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passwordCnf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expectedRes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">please fill out this filled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABCDEFGH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyz12345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#$%++++#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please enter a valid username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12345xyz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xyz1234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password should contain atleast 8 characters </t>
+  </si>
+  <si>
+    <t xml:space="preserve">12345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password should contain character with number </t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Account Created. You are logged in as abcd1234 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -136,7 +203,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -149,8 +216,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -230,10 +309,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -252,45 +331,90 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="Pwd@1234"/>
-    <hyperlink ref="B3" r:id="rId2" display="Pwd@12345"/>
-    <hyperlink ref="B4" r:id="rId3" display="Pwd@1234"/>
+    <hyperlink ref="B4" r:id="rId2" display="Pwd@12345"/>
+    <hyperlink ref="B5" r:id="rId3" display="Pwd@1234"/>
+    <hyperlink ref="B6" r:id="rId4" display="Pwd@12345"/>
+    <hyperlink ref="B7" r:id="rId5" display="Pwd@1234"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -307,14 +431,158 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="5" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="49.37"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="5" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>